<commit_message>
update mortality_table.py to print the object and create the example for the manual
</commit_message>
<xml_diff>
--- a/exercisesLifeContingencies/survivalModels/lifeTables3/GRF_95.xlsx
+++ b/exercisesLifeContingencies/survivalModels/lifeTables3/GRF_95.xlsx
@@ -1,37 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="GRF_95" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="GRF_95" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>lx</t>
+  </si>
+  <si>
+    <t>dx</t>
+  </si>
+  <si>
+    <t>qx</t>
+  </si>
+  <si>
+    <t>px</t>
+  </si>
+  <si>
+    <t>exo</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +72,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,2595 +388,2579 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>lx</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>dx</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>qx</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>px</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>exo</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>100000</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>89.30480517450458</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:6">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>100000</v>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>88.30480517450458</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:6">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>100000</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>87.30480517450459</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:6">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>100000</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>86.30480517450458</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:6">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>100000</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>85.30480517450458</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:6">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>100000</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>84.30480517450457</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:6">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>100000</v>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>83.30480517450458</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" spans="1:6">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>100000</v>
       </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>82.30480517450455</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" spans="1:6">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>100000</v>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>81.30480517450455</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="11" spans="1:6">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>100000</v>
       </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>80.30480517450455</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
+    <row r="12" spans="1:6">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>100000</v>
       </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>79.30480517450455</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
+    <row r="13" spans="1:6">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>100000</v>
       </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>78.30480517450455</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n">
+    <row r="14" spans="1:6">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>100000</v>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="n">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>77.30480517450455</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
+    <row r="15" spans="1:6">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>100000</v>
       </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="n">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>76.30480517450455</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="n">
+    <row r="16" spans="1:6">
+      <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>100000</v>
       </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" t="n">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>75.30480517450455</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="n">
+    <row r="17" spans="1:6">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>100000</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>31.79</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>0.0003179</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>0.9996821</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17">
         <v>74.30480517450454</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="n">
+    <row r="18" spans="1:6">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>99968.21000000001</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>31.979830379</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>0.0003199</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>0.9996801</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18">
         <v>73.32827518318526</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="n">
+    <row r="19" spans="1:6">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>99936.23016962101</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19">
         <v>32.16947249160101</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>0.0003219</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>0.9996781</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19">
         <v>72.35158040375643</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="n">
+    <row r="20" spans="1:6">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>99904.0606971294</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>32.35892525980022</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>0.0003239</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>0.9996761</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20">
         <v>71.37471687511851</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="n">
+    <row r="21" spans="1:6">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>99871.7017718696</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>32.54818760745231</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>0.0003259</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>0.9996741</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21">
         <v>70.39768063387584</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="n">
+    <row r="22" spans="1:6">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>99839.15358426215</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>32.80714586778854</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>0.0003286</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>0.9996714</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22">
         <v>69.42046771430392</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="n">
+    <row r="23" spans="1:6">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>99806.34643839436</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23">
         <v>34.17369302050623</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23">
         <v>0.0003424</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>0.9996576</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23">
         <v>68.44312242433257</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="n">
+    <row r="24" spans="1:6">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>99772.17274537386</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24">
         <v>36.55652409390498</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>0.0003664</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>0.9996336</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24">
         <v>67.46639411767846</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="n">
+    <row r="25" spans="1:6">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>99735.61622127995</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25">
         <v>39.42548909227197</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25">
         <v>0.0003953</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25">
         <v>0.9996047</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25">
         <v>66.49093959794715</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="n">
+    <row r="26" spans="1:6">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>99696.19073218768</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26">
         <v>42.34097220396011</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26">
         <v>0.0004247</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26">
         <v>0.9995753000000001</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26">
         <v>65.51703613233025</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="n">
+    <row r="27" spans="1:6">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>99653.84975998373</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>45.25281317600861</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27">
         <v>0.0004541</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27">
         <v>0.9995459</v>
       </c>
-      <c r="F27" t="n">
+      <c r="F27">
         <v>64.54466059968694</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="n">
+    <row r="28" spans="1:6">
+      <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>99608.59694680772</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28">
         <v>48.20060006256026</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28">
         <v>0.0004839</v>
       </c>
-      <c r="E28" t="n">
+      <c r="E28">
         <v>0.9995161</v>
       </c>
-      <c r="F28" t="n">
+      <c r="F28">
         <v>63.57375649251018</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="n">
+    <row r="29" spans="1:6">
+      <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>99560.39634674517</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29">
         <v>51.20391184113104</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29">
         <v>0.0005143</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E29">
         <v>0.9994857</v>
       </c>
-      <c r="F29" t="n">
+      <c r="F29">
         <v>62.60429265972822</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="n">
+    <row r="30" spans="1:6">
+      <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>99509.19243490403</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30">
         <v>54.29221539248365</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30">
         <v>0.0005456</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E30">
         <v>0.9994544</v>
       </c>
-      <c r="F30" t="n">
+      <c r="F30">
         <v>61.63624933276007</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="n">
+    <row r="31" spans="1:6">
+      <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>99454.90021951155</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31">
         <v>57.51476879694353</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31">
         <v>0.0005783</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E31">
         <v>0.9994217</v>
       </c>
-      <c r="F31" t="n">
+      <c r="F31">
         <v>60.66962347933038</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="n">
+    <row r="32" spans="1:6">
+      <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>99397.3854507146</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32">
         <v>60.87095885001762</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32">
         <v>0.0006124</v>
       </c>
-      <c r="E32" t="n">
+      <c r="E32">
         <v>0.9993876</v>
       </c>
-      <c r="F32" t="n">
+      <c r="F32">
         <v>59.70443970681284</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="n">
+    <row r="33" spans="1:6">
+      <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>99336.51449186458</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33">
         <v>64.41972964797418</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33">
         <v>0.0006485</v>
       </c>
-      <c r="E33" t="n">
+      <c r="E33">
         <v>0.9993514999999999</v>
       </c>
-      <c r="F33" t="n">
+      <c r="F33">
         <v>58.74071872295878</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="n">
+    <row r="34" spans="1:6">
+      <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>99272.0947622166</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34">
         <v>68.17014747321414</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34">
         <v>0.0006867</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E34">
         <v>0.9993133</v>
       </c>
-      <c r="F34" t="n">
+      <c r="F34">
         <v>57.77851233821013</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="n">
+    <row r="35" spans="1:6">
+      <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>99203.92461474337</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35">
         <v>72.16093476476433</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35">
         <v>0.0007274</v>
       </c>
-      <c r="E35" t="n">
+      <c r="E35">
         <v>0.9992726</v>
       </c>
-      <c r="F35" t="n">
+      <c r="F35">
         <v>56.81787252127049</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="n">
+    <row r="36" spans="1:6">
+      <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>99131.7636799786</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36">
         <v>76.42067662089551</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36">
         <v>0.0007709</v>
       </c>
-      <c r="E36" t="n">
+      <c r="E36">
         <v>0.9992291</v>
       </c>
-      <c r="F36" t="n">
+      <c r="F36">
         <v>55.85886796182592</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="n">
+    <row r="37" spans="1:6">
+      <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>99055.3430033577</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37">
         <v>80.96783737094459</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37">
         <v>0.0008174</v>
       </c>
-      <c r="E37" t="n">
+      <c r="E37">
         <v>0.9991826</v>
       </c>
-      <c r="F37" t="n">
+      <c r="F37">
         <v>54.90157703756418</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="n">
+    <row r="38" spans="1:6">
+      <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>98974.37516598676</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38">
         <v>85.82068070642711</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38">
         <v>0.0008671</v>
       </c>
-      <c r="E38" t="n">
+      <c r="E38">
         <v>0.9991329</v>
       </c>
-      <c r="F38" t="n">
+      <c r="F38">
         <v>53.94608126438969</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="n">
+    <row r="39" spans="1:6">
+      <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>98888.55448528033</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39">
         <v>90.89835928286968</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39">
         <v>0.0009192</v>
       </c>
-      <c r="E39" t="n">
+      <c r="E39">
         <v>0.9990808</v>
       </c>
-      <c r="F39" t="n">
+      <c r="F39">
         <v>52.9924645804274</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="n">
+    <row r="40" spans="1:6">
+      <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>98797.65612599746</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40">
         <v>96.13011941059553</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40">
         <v>0.000973</v>
       </c>
-      <c r="E40" t="n">
+      <c r="E40">
         <v>0.999027</v>
       </c>
-      <c r="F40" t="n">
+      <c r="F40">
         <v>52.04076004706265</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="n">
+    <row r="41" spans="1:6">
+      <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>98701.52600658686</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41">
         <v>101.4355582769693</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41">
         <v>0.0010277</v>
       </c>
-      <c r="E41" t="n">
+      <c r="E41">
         <v>0.9989723</v>
       </c>
-      <c r="F41" t="n">
+      <c r="F41">
         <v>51.09095804924456</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="n">
+    <row r="42" spans="1:6">
+      <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>98600.0904483099</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42">
         <v>106.705017883161</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42">
         <v>0.0010822</v>
       </c>
-      <c r="E42" t="n">
+      <c r="E42">
         <v>0.9989178</v>
       </c>
-      <c r="F42" t="n">
+      <c r="F42">
         <v>50.14300386431592</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="n">
+    <row r="43" spans="1:6">
+      <c r="A43">
         <v>41</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>98493.38543042673</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43">
         <v>111.8884858489648</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43">
         <v>0.001136</v>
       </c>
-      <c r="E43" t="n">
+      <c r="E43">
         <v>0.998864</v>
       </c>
-      <c r="F43" t="n">
+      <c r="F43">
         <v>49.19678572582842</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="n">
+    <row r="44" spans="1:6">
+      <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>98381.49694457777</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44">
         <v>116.8772183701584</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D44">
         <v>0.001188</v>
       </c>
-      <c r="E44" t="n">
+      <c r="E44">
         <v>0.998812</v>
       </c>
-      <c r="F44" t="n">
+      <c r="F44">
         <v>48.25216818889098</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="n">
+    <row r="45" spans="1:6">
+      <c r="A45">
         <v>43</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>98264.61972620762</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45">
         <v>121.6909050689355</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D45">
         <v>0.0012384</v>
       </c>
-      <c r="E45" t="n">
+      <c r="E45">
         <v>0.9987616</v>
       </c>
-      <c r="F45" t="n">
+      <c r="F45">
         <v>47.30896523959562</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="n">
+    <row r="46" spans="1:6">
+      <c r="A46">
         <v>44</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>98142.92882113869</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46">
         <v>126.6436353507974</v>
       </c>
-      <c r="D46" t="n">
+      <c r="D46">
         <v>0.0012904</v>
       </c>
-      <c r="E46" t="n">
+      <c r="E46">
         <v>0.9987096</v>
       </c>
-      <c r="F46" t="n">
+      <c r="F46">
         <v>46.36700533900743</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="n">
+    <row r="47" spans="1:6">
+      <c r="A47">
         <v>45</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>98016.28518578788</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47">
         <v>132.1651589445164</v>
       </c>
-      <c r="D47" t="n">
+      <c r="D47">
         <v>0.0013484</v>
       </c>
-      <c r="E47" t="n">
+      <c r="E47">
         <v>0.9986516</v>
       </c>
-      <c r="F47" t="n">
+      <c r="F47">
         <v>45.42626859600373</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="n">
+    <row r="48" spans="1:6">
+      <c r="A48">
         <v>46</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>97884.12002684336</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48">
         <v>138.6332791940182</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48">
         <v>0.0014163</v>
       </c>
-      <c r="E48" t="n">
+      <c r="E48">
         <v>0.9985837</v>
       </c>
-      <c r="F48" t="n">
+      <c r="F48">
         <v>44.48692897102826</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="n">
+    <row r="49" spans="1:6">
+      <c r="A49">
         <v>47</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>97745.48674764934</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49">
         <v>145.7971680327938</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D49">
         <v>0.0014916</v>
       </c>
-      <c r="E49" t="n">
+      <c r="E49">
         <v>0.9985084</v>
       </c>
-      <c r="F49" t="n">
+      <c r="F49">
         <v>43.54931601730357</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="n">
+    <row r="50" spans="1:6">
+      <c r="A50">
         <v>48</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>97599.68957961653</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50">
         <v>153.2119927020821</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50">
         <v>0.0015698</v>
       </c>
-      <c r="E50" t="n">
+      <c r="E50">
         <v>0.9984302</v>
       </c>
-      <c r="F50" t="n">
+      <c r="F50">
         <v>42.61362429930846</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="n">
+    <row r="51" spans="1:6">
+      <c r="A51">
         <v>49</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>97446.47758691445</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51">
         <v>161.0400488601348</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D51">
         <v>0.0016526</v>
       </c>
-      <c r="E51" t="n">
+      <c r="E51">
         <v>0.9983474</v>
       </c>
-      <c r="F51" t="n">
+      <c r="F51">
         <v>41.67983820932946</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="n">
+    <row r="52" spans="1:6">
+      <c r="A52">
         <v>50</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>97285.43753805432</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52">
         <v>169.4420465600292</v>
       </c>
-      <c r="D52" t="n">
+      <c r="D52">
         <v>0.0017417</v>
       </c>
-      <c r="E52" t="n">
+      <c r="E52">
         <v>0.9982583</v>
       </c>
-      <c r="F52" t="n">
+      <c r="F52">
         <v>40.7480046618336</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="n">
+    <row r="53" spans="1:6">
+      <c r="A53">
         <v>51</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>97115.99549149429</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53">
         <v>178.5671809102106</v>
       </c>
-      <c r="D53" t="n">
+      <c r="D53">
         <v>0.0018387</v>
       </c>
-      <c r="E53" t="n">
+      <c r="E53">
         <v>0.9981613</v>
       </c>
-      <c r="F53" t="n">
+      <c r="F53">
         <v>39.81822691765608</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="n">
+    <row r="54" spans="1:6">
+      <c r="A54">
         <v>52</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54">
         <v>96937.42831058409</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54">
         <v>188.5723792925792</v>
       </c>
-      <c r="D54" t="n">
+      <c r="D54">
         <v>0.0019453</v>
       </c>
-      <c r="E54" t="n">
+      <c r="E54">
         <v>0.9980547</v>
       </c>
-      <c r="F54" t="n">
+      <c r="F54">
         <v>38.89065451411118</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="n">
+    <row r="55" spans="1:6">
+      <c r="A55">
         <v>53</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55">
         <v>96748.8559312915</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C55">
         <v>199.6219144430338</v>
       </c>
-      <c r="D55" t="n">
+      <c r="D55">
         <v>0.0020633</v>
       </c>
-      <c r="E55" t="n">
+      <c r="E55">
         <v>0.9979367</v>
       </c>
-      <c r="F55" t="n">
+      <c r="F55">
         <v>37.96548141510799</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="n">
+    <row r="56" spans="1:6">
+      <c r="A56">
         <v>54</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56">
         <v>96549.23401684847</v>
       </c>
-      <c r="C56" t="n">
+      <c r="C56">
         <v>211.8386743563672</v>
       </c>
-      <c r="D56" t="n">
+      <c r="D56">
         <v>0.0021941</v>
       </c>
-      <c r="E56" t="n">
+      <c r="E56">
         <v>0.9978059</v>
       </c>
-      <c r="F56" t="n">
+      <c r="F56">
         <v>37.04294377099068</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="n">
+    <row r="57" spans="1:6">
+      <c r="A57">
         <v>55</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57">
         <v>96337.39534249211</v>
       </c>
-      <c r="C57" t="n">
+      <c r="C57">
         <v>225.3909701432945</v>
       </c>
-      <c r="D57" t="n">
+      <c r="D57">
         <v>0.0023396</v>
       </c>
-      <c r="E57" t="n">
+      <c r="E57">
         <v>0.9976604</v>
       </c>
-      <c r="F57" t="n">
+      <c r="F57">
         <v>36.12329895121954</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="n">
+    <row r="58" spans="1:6">
+      <c r="A58">
         <v>56</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58">
         <v>96112.00437234881</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58">
         <v>240.4145677369933</v>
       </c>
-      <c r="D58" t="n">
+      <c r="D58">
         <v>0.0025014</v>
       </c>
-      <c r="E58" t="n">
+      <c r="E58">
         <v>0.9974986</v>
       </c>
-      <c r="F58" t="n">
+      <c r="F58">
         <v>35.20683867097415</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="n">
+    <row r="59" spans="1:6">
+      <c r="A59">
         <v>57</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59">
         <v>95871.58980461181</v>
       </c>
-      <c r="C59" t="n">
+      <c r="C59">
         <v>257.0413194251447</v>
       </c>
-      <c r="D59" t="n">
+      <c r="D59">
         <v>0.0026811</v>
       </c>
-      <c r="E59" t="n">
+      <c r="E59">
         <v>0.9973189</v>
       </c>
-      <c r="F59" t="n">
+      <c r="F59">
         <v>34.29387206255142</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="n">
+    <row r="60" spans="1:6">
+      <c r="A60">
         <v>58</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60">
         <v>95614.54848518666</v>
       </c>
-      <c r="C60" t="n">
+      <c r="C60">
         <v>275.4177069115802</v>
       </c>
-      <c r="D60" t="n">
+      <c r="D60">
         <v>0.0028805</v>
       </c>
-      <c r="E60" t="n">
+      <c r="E60">
         <v>0.9971195</v>
       </c>
-      <c r="F60" t="n">
+      <c r="F60">
         <v>33.38472038637934</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="n">
+    <row r="61" spans="1:6">
+      <c r="A61">
         <v>59</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61">
         <v>95339.1307782751</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C61">
         <v>295.6657123695867</v>
       </c>
-      <c r="D61" t="n">
+      <c r="D61">
         <v>0.0031012</v>
       </c>
-      <c r="E61" t="n">
+      <c r="E61">
         <v>0.9968988</v>
       </c>
-      <c r="F61" t="n">
+      <c r="F61">
         <v>32.47971846541897</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="n">
+    <row r="62" spans="1:6">
+      <c r="A62">
         <v>60</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62">
         <v>95043.4650659055</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C62">
         <v>317.9013819524408</v>
       </c>
-      <c r="D62" t="n">
+      <c r="D62">
         <v>0.0033448</v>
       </c>
-      <c r="E62" t="n">
+      <c r="E62">
         <v>0.9966552</v>
       </c>
-      <c r="F62" t="n">
+      <c r="F62">
         <v>31.5792024881753</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="n">
+    <row r="63" spans="1:6">
+      <c r="A63">
         <v>61</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B63">
         <v>94725.56368395306</v>
       </c>
-      <c r="C63" t="n">
+      <c r="C63">
         <v>340.197389414549</v>
       </c>
-      <c r="D63" t="n">
+      <c r="D63">
         <v>0.0035914</v>
       </c>
-      <c r="E63" t="n">
+      <c r="E63">
         <v>0.9964086</v>
       </c>
-      <c r="F63" t="n">
+      <c r="F63">
         <v>30.68350507595335</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="n">
+    <row r="64" spans="1:6">
+      <c r="A64">
         <v>62</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B64">
         <v>94385.36629453851</v>
       </c>
-      <c r="C64" t="n">
+      <c r="C64">
         <v>362.6002616937286</v>
       </c>
-      <c r="D64" t="n">
+      <c r="D64">
         <v>0.0038417</v>
       </c>
-      <c r="E64" t="n">
+      <c r="E64">
         <v>0.9961583000000001</v>
       </c>
-      <c r="F64" t="n">
+      <c r="F64">
         <v>29.79229683079146</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="n">
+    <row r="65" spans="1:6">
+      <c r="A65">
         <v>63</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B65">
         <v>94022.7660328448</v>
       </c>
-      <c r="C65" t="n">
+      <c r="C65">
         <v>387.9755417579307</v>
       </c>
-      <c r="D65" t="n">
+      <c r="D65">
         <v>0.0041264</v>
       </c>
-      <c r="E65" t="n">
+      <c r="E65">
         <v>0.9958736</v>
       </c>
-      <c r="F65" t="n">
+      <c r="F65">
         <v>28.90526302977294</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" t="n">
+    <row r="66" spans="1:6">
+      <c r="A66">
         <v>64</v>
       </c>
-      <c r="B66" t="n">
+      <c r="B66">
         <v>93634.79049108687</v>
       </c>
-      <c r="C66" t="n">
+      <c r="C66">
         <v>418.8752352618771</v>
       </c>
-      <c r="D66" t="n">
+      <c r="D66">
         <v>0.0044735</v>
       </c>
-      <c r="E66" t="n">
+      <c r="E66">
         <v>0.9955265</v>
       </c>
-      <c r="F66" t="n">
+      <c r="F66">
         <v>28.02296017262927</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" t="n">
+    <row r="67" spans="1:6">
+      <c r="A67">
         <v>65</v>
       </c>
-      <c r="B67" t="n">
+      <c r="B67">
         <v>93215.91525582499</v>
       </c>
-      <c r="C67" t="n">
+      <c r="C67">
         <v>457.5596416247425</v>
       </c>
-      <c r="D67" t="n">
+      <c r="D67">
         <v>0.0049086</v>
       </c>
-      <c r="E67" t="n">
+      <c r="E67">
         <v>0.9950914</v>
       </c>
-      <c r="F67" t="n">
+      <c r="F67">
         <v>27.14663740506081</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="n">
+    <row r="68" spans="1:6">
+      <c r="A68">
         <v>66</v>
       </c>
-      <c r="B68" t="n">
+      <c r="B68">
         <v>92758.35561420025</v>
       </c>
-      <c r="C68" t="n">
+      <c r="C68">
         <v>505.3846247284087</v>
       </c>
-      <c r="D68" t="n">
+      <c r="D68">
         <v>0.0054484</v>
       </c>
-      <c r="E68" t="n">
+      <c r="E68">
         <v>0.9945516</v>
       </c>
-      <c r="F68" t="n">
+      <c r="F68">
         <v>26.27808028997217</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" t="n">
+    <row r="69" spans="1:6">
+      <c r="A69">
         <v>67</v>
       </c>
-      <c r="B69" t="n">
+      <c r="B69">
         <v>92252.97098947184</v>
       </c>
-      <c r="C69" t="n">
+      <c r="C69">
         <v>561.1471466376604</v>
       </c>
-      <c r="D69" t="n">
+      <c r="D69">
         <v>0.0060827</v>
       </c>
-      <c r="E69" t="n">
+      <c r="E69">
         <v>0.9939173</v>
       </c>
-      <c r="F69" t="n">
+      <c r="F69">
         <v>25.41929899863634</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="n">
+    <row r="70" spans="1:6">
+      <c r="A70">
         <v>68</v>
       </c>
-      <c r="B70" t="n">
+      <c r="B70">
         <v>91691.82384283419</v>
       </c>
-      <c r="C70" t="n">
+      <c r="C70">
         <v>623.0826197415954</v>
       </c>
-      <c r="D70" t="n">
+      <c r="D70">
         <v>0.0067954</v>
       </c>
-      <c r="E70" t="n">
+      <c r="E70">
         <v>0.9932046</v>
       </c>
-      <c r="F70" t="n">
+      <c r="F70">
         <v>24.57180325630345</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="n">
+    <row r="71" spans="1:6">
+      <c r="A71">
         <v>69</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B71">
         <v>91068.74122309258</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C71">
         <v>689.5634016671347</v>
       </c>
-      <c r="D71" t="n">
+      <c r="D71">
         <v>0.0075719</v>
       </c>
-      <c r="E71" t="n">
+      <c r="E71">
         <v>0.9924281</v>
       </c>
-      <c r="F71" t="n">
+      <c r="F71">
         <v>23.73649996818729</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="n">
+    <row r="72" spans="1:6">
+      <c r="A72">
         <v>70</v>
       </c>
-      <c r="B72" t="n">
+      <c r="B72">
         <v>90379.17782142546</v>
       </c>
-      <c r="C72" t="n">
+      <c r="C72">
         <v>759.0404870154596</v>
       </c>
-      <c r="D72" t="n">
+      <c r="D72">
         <v>0.0083984</v>
       </c>
-      <c r="E72" t="n">
+      <c r="E72">
         <v>0.9916016</v>
       </c>
-      <c r="F72" t="n">
+      <c r="F72">
         <v>22.91378682061429</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="n">
+    <row r="73" spans="1:6">
+      <c r="A73">
         <v>71</v>
       </c>
-      <c r="B73" t="n">
+      <c r="B73">
         <v>89620.13733441</v>
       </c>
-      <c r="C73" t="n">
+      <c r="C73">
         <v>830.0527499775719</v>
       </c>
-      <c r="D73" t="n">
+      <c r="D73">
         <v>0.0092619</v>
       </c>
-      <c r="E73" t="n">
+      <c r="E73">
         <v>0.9907381</v>
       </c>
-      <c r="F73" t="n">
+      <c r="F73">
         <v>22.1036210718239</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" t="n">
+    <row r="74" spans="1:6">
+      <c r="A74">
         <v>72</v>
       </c>
-      <c r="B74" t="n">
+      <c r="B74">
         <v>88790.08458443242</v>
       </c>
-      <c r="C74" t="n">
+      <c r="C74">
         <v>901.2815115911982</v>
       </c>
-      <c r="D74" t="n">
+      <c r="D74">
         <v>0.0101507</v>
       </c>
-      <c r="E74" t="n">
+      <c r="E74">
         <v>0.9898493</v>
       </c>
-      <c r="F74" t="n">
+      <c r="F74">
         <v>21.30558219354227</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="n">
+    <row r="75" spans="1:6">
+      <c r="A75">
         <v>73</v>
       </c>
-      <c r="B75" t="n">
+      <c r="B75">
         <v>87888.80307284123</v>
       </c>
-      <c r="C75" t="n">
+      <c r="C75">
         <v>971.5052514065724</v>
       </c>
-      <c r="D75" t="n">
+      <c r="D75">
         <v>0.0110538</v>
       </c>
-      <c r="E75" t="n">
+      <c r="E75">
         <v>0.9889462</v>
       </c>
-      <c r="F75" t="n">
+      <c r="F75">
         <v>20.51893913906113</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="n">
+    <row r="76" spans="1:6">
+      <c r="A76">
         <v>74</v>
       </c>
-      <c r="B76" t="n">
+      <c r="B76">
         <v>86917.29782143465</v>
       </c>
-      <c r="C76" t="n">
+      <c r="C76">
         <v>1039.61779924218</v>
       </c>
-      <c r="D76" t="n">
+      <c r="D76">
         <v>0.011961</v>
       </c>
-      <c r="E76" t="n">
+      <c r="E76">
         <v>0.988039</v>
       </c>
-      <c r="F76" t="n">
+      <c r="F76">
         <v>19.74269787280758</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" t="n">
+    <row r="77" spans="1:6">
+      <c r="A77">
         <v>75</v>
       </c>
-      <c r="B77" t="n">
+      <c r="B77">
         <v>85877.68002219248</v>
       </c>
-      <c r="C77" t="n">
+      <c r="C77">
         <v>1105.91558778979</v>
       </c>
-      <c r="D77" t="n">
+      <c r="D77">
         <v>0.0128778</v>
       </c>
-      <c r="E77" t="n">
+      <c r="E77">
         <v>0.9871221999999999</v>
       </c>
-      <c r="F77" t="n">
+      <c r="F77">
         <v>18.97564607551683</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="n">
+    <row r="78" spans="1:6">
+      <c r="A78">
         <v>76</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B78">
         <v>84771.76443440268</v>
       </c>
-      <c r="C78" t="n">
+      <c r="C78">
         <v>1175.62330635274</v>
       </c>
-      <c r="D78" t="n">
+      <c r="D78">
         <v>0.0138681</v>
       </c>
-      <c r="E78" t="n">
+      <c r="E78">
         <v>0.9861319</v>
       </c>
-      <c r="F78" t="n">
+      <c r="F78">
         <v>18.21667568160946</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="n">
+    <row r="79" spans="1:6">
+      <c r="A79">
         <v>77</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B79">
         <v>83596.14112804993</v>
       </c>
-      <c r="C79" t="n">
+      <c r="C79">
         <v>1254.284861099374</v>
       </c>
-      <c r="D79" t="n">
+      <c r="D79">
         <v>0.0150041</v>
       </c>
-      <c r="E79" t="n">
+      <c r="E79">
         <v>0.9849959</v>
       </c>
-      <c r="F79" t="n">
+      <c r="F79">
         <v>17.46582757500235</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" t="n">
+    <row r="80" spans="1:6">
+      <c r="A80">
         <v>78</v>
       </c>
-      <c r="B80" t="n">
+      <c r="B80">
         <v>82341.85626695056</v>
       </c>
-      <c r="C80" t="n">
+      <c r="C80">
         <v>1346.454033677175</v>
       </c>
-      <c r="D80" t="n">
+      <c r="D80">
         <v>0.016352</v>
       </c>
-      <c r="E80" t="n">
+      <c r="E80">
         <v>0.983648</v>
       </c>
-      <c r="F80" t="n">
+      <c r="F80">
         <v>16.72426212637266</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" t="n">
+    <row r="81" spans="1:6">
+      <c r="A81">
         <v>79</v>
       </c>
-      <c r="B81" t="n">
+      <c r="B81">
         <v>80995.40223327339</v>
       </c>
-      <c r="C81" t="n">
+      <c r="C81">
         <v>1455.616970775496</v>
       </c>
-      <c r="D81" t="n">
+      <c r="D81">
         <v>0.0179716</v>
       </c>
-      <c r="E81" t="n">
+      <c r="E81">
         <v>0.9820284</v>
       </c>
-      <c r="F81" t="n">
+      <c r="F81">
         <v>15.99397154914427</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" t="n">
+    <row r="82" spans="1:6">
+      <c r="A82">
         <v>80</v>
       </c>
-      <c r="B82" t="n">
+      <c r="B82">
         <v>79539.7852624979</v>
       </c>
-      <c r="C82" t="n">
+      <c r="C82">
         <v>1584.201857051697</v>
       </c>
-      <c r="D82" t="n">
+      <c r="D82">
         <v>0.0199171</v>
       </c>
-      <c r="E82" t="n">
+      <c r="E82">
         <v>0.9800829</v>
       </c>
-      <c r="F82" t="n">
+      <c r="F82">
         <v>15.27751880612034</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" t="n">
+    <row r="83" spans="1:6">
+      <c r="A83">
         <v>81</v>
       </c>
-      <c r="B83" t="n">
+      <c r="B83">
         <v>77955.5834054462</v>
       </c>
-      <c r="C83" t="n">
+      <c r="C83">
         <v>1733.513899303588</v>
       </c>
-      <c r="D83" t="n">
+      <c r="D83">
         <v>0.0222372</v>
       </c>
-      <c r="E83" t="n">
+      <c r="E83">
         <v>0.9777628</v>
       </c>
-      <c r="F83" t="n">
+      <c r="F83">
         <v>14.57782536163046</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" t="n">
+    <row r="84" spans="1:6">
+      <c r="A84">
         <v>82</v>
       </c>
-      <c r="B84" t="n">
+      <c r="B84">
         <v>76222.06950614262</v>
       </c>
-      <c r="C84" t="n">
+      <c r="C84">
         <v>1903.684296950665</v>
       </c>
-      <c r="D84" t="n">
+      <c r="D84">
         <v>0.0249755</v>
       </c>
-      <c r="E84" t="n">
+      <c r="E84">
         <v>0.9750245</v>
       </c>
-      <c r="F84" t="n">
+      <c r="F84">
         <v>13.89799648915919</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" t="n">
+    <row r="85" spans="1:6">
+      <c r="A85">
         <v>83</v>
       </c>
-      <c r="B85" t="n">
+      <c r="B85">
         <v>74318.38520919195</v>
       </c>
-      <c r="C85" t="n">
+      <c r="C85">
         <v>2092.233475924735</v>
       </c>
-      <c r="D85" t="n">
+      <c r="D85">
         <v>0.0281523</v>
       </c>
-      <c r="E85" t="n">
+      <c r="E85">
         <v>0.9718477</v>
       </c>
-      <c r="F85" t="n">
+      <c r="F85">
         <v>13.24118956924589</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" t="n">
+    <row r="86" spans="1:6">
+      <c r="A86">
         <v>84</v>
       </c>
-      <c r="B86" t="n">
+      <c r="B86">
         <v>72226.15173326722</v>
       </c>
-      <c r="C86" t="n">
+      <c r="C86">
         <v>2290.536840377797</v>
       </c>
-      <c r="D86" t="n">
+      <c r="D86">
         <v>0.0317134</v>
       </c>
-      <c r="E86" t="n">
+      <c r="E86">
         <v>0.9682866</v>
       </c>
-      <c r="F86" t="n">
+      <c r="F86">
         <v>12.61027393412146</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" t="n">
+    <row r="87" spans="1:6">
+      <c r="A87">
         <v>85</v>
       </c>
-      <c r="B87" t="n">
+      <c r="B87">
         <v>69935.61489288943</v>
       </c>
-      <c r="C87" t="n">
+      <c r="C87">
         <v>2489.043501845381</v>
       </c>
-      <c r="D87" t="n">
+      <c r="D87">
         <v>0.0355905</v>
       </c>
-      <c r="E87" t="n">
+      <c r="E87">
         <v>0.9644095</v>
       </c>
-      <c r="F87" t="n">
+      <c r="F87">
         <v>12.00691059250583</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" t="n">
+    <row r="88" spans="1:6">
+      <c r="A88">
         <v>86</v>
       </c>
-      <c r="B88" t="n">
+      <c r="B88">
         <v>67446.57139104405</v>
       </c>
-      <c r="C88" t="n">
+      <c r="C88">
         <v>2678.950837023714</v>
       </c>
-      <c r="D88" t="n">
+      <c r="D88">
         <v>0.0397196</v>
       </c>
-      <c r="E88" t="n">
+      <c r="E88">
         <v>0.9602804</v>
       </c>
-      <c r="F88" t="n">
+      <c r="F88">
         <v>11.4315608074224</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" t="n">
+    <row r="89" spans="1:6">
+      <c r="A89">
         <v>87</v>
       </c>
-      <c r="B89" t="n">
+      <c r="B89">
         <v>64767.62055402034</v>
       </c>
-      <c r="C89" t="n">
+      <c r="C89">
         <v>2852.463160629887</v>
       </c>
-      <c r="D89" t="n">
+      <c r="D89">
         <v>0.0440415</v>
       </c>
-      <c r="E89" t="n">
+      <c r="E89">
         <v>0.9559585</v>
       </c>
-      <c r="F89" t="n">
+      <c r="F89">
         <v>10.88371751357457</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" t="n">
+    <row r="90" spans="1:6">
+      <c r="A90">
         <v>88</v>
       </c>
-      <c r="B90" t="n">
+      <c r="B90">
         <v>61915.15739339046</v>
       </c>
-      <c r="C90" t="n">
+      <c r="C90">
         <v>3002.95324025257</v>
       </c>
-      <c r="D90" t="n">
+      <c r="D90">
         <v>0.0485011</v>
       </c>
-      <c r="E90" t="n">
+      <c r="E90">
         <v>0.9514989</v>
       </c>
-      <c r="F90" t="n">
+      <c r="F90">
         <v>10.36210072254661</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" t="n">
+    <row r="91" spans="1:6">
+      <c r="A91">
         <v>89</v>
       </c>
-      <c r="B91" t="n">
+      <c r="B91">
         <v>58912.20415313789</v>
       </c>
-      <c r="C91" t="n">
+      <c r="C91">
         <v>3125.139258593167</v>
       </c>
-      <c r="D91" t="n">
+      <c r="D91">
         <v>0.0530474</v>
       </c>
-      <c r="E91" t="n">
+      <c r="E91">
         <v>0.9469526</v>
       </c>
-      <c r="F91" t="n">
+      <c r="F91">
         <v>9.864805174810616</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" t="n">
+    <row r="92" spans="1:6">
+      <c r="A92">
         <v>90</v>
       </c>
-      <c r="B92" t="n">
+      <c r="B92">
         <v>55787.06489454472</v>
       </c>
-      <c r="C92" t="n">
+      <c r="C92">
         <v>3215.175911067296</v>
       </c>
-      <c r="D92" t="n">
+      <c r="D92">
         <v>0.057633</v>
       </c>
-      <c r="E92" t="n">
+      <c r="E92">
         <v>0.942367</v>
       </c>
-      <c r="F92" t="n">
+      <c r="F92">
         <v>9.389412812014688</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" t="n">
+    <row r="93" spans="1:6">
+      <c r="A93">
         <v>91</v>
       </c>
-      <c r="B93" t="n">
+      <c r="B93">
         <v>52571.88898347742</v>
       </c>
-      <c r="C93" t="n">
+      <c r="C93">
         <v>3270.728529973658</v>
       </c>
-      <c r="D93" t="n">
+      <c r="D93">
         <v>0.0622144</v>
       </c>
-      <c r="E93" t="n">
+      <c r="E93">
         <v>0.9377856</v>
       </c>
-      <c r="F93" t="n">
+      <c r="F93">
         <v>8.933068870211594</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" t="n">
+    <row r="94" spans="1:6">
+      <c r="A94">
         <v>92</v>
       </c>
-      <c r="B94" t="n">
+      <c r="B94">
         <v>49301.16045350376</v>
       </c>
-      <c r="C94" t="n">
+      <c r="C94">
         <v>3293.559093980274</v>
       </c>
-      <c r="D94" t="n">
+      <c r="D94">
         <v>0.0668049</v>
       </c>
-      <c r="E94" t="n">
+      <c r="E94">
         <v>0.9331951000000001</v>
       </c>
-      <c r="F94" t="n">
+      <c r="F94">
         <v>8.492533976008584</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" t="n">
+    <row r="95" spans="1:6">
+      <c r="A95">
         <v>93</v>
       </c>
-      <c r="B95" t="n">
+      <c r="B95">
         <v>46007.60135952349</v>
       </c>
-      <c r="C95" t="n">
+      <c r="C95">
         <v>3295.345055737365</v>
       </c>
-      <c r="D95" t="n">
+      <c r="D95">
         <v>0.0716261</v>
       </c>
-      <c r="E95" t="n">
+      <c r="E95">
         <v>0.9283739</v>
       </c>
-      <c r="F95" t="n">
+      <c r="F95">
         <v>8.064697752922815</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="n">
+    <row r="96" spans="1:6">
+      <c r="A96">
         <v>94</v>
       </c>
-      <c r="B96" t="n">
+      <c r="B96">
         <v>42712.25630378613</v>
       </c>
-      <c r="C96" t="n">
+      <c r="C96">
         <v>3285.922217060353</v>
       </c>
-      <c r="D96" t="n">
+      <c r="D96">
         <v>0.0769316</v>
       </c>
-      <c r="E96" t="n">
+      <c r="E96">
         <v>0.9230684</v>
       </c>
-      <c r="F96" t="n">
+      <c r="F96">
         <v>7.648330918095409</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" t="n">
+    <row r="97" spans="1:6">
+      <c r="A97">
         <v>95</v>
       </c>
-      <c r="B97" t="n">
+      <c r="B97">
         <v>39426.33408672577</v>
       </c>
-      <c r="C97" t="n">
+      <c r="C97">
         <v>3270.509035695711</v>
       </c>
-      <c r="D97" t="n">
+      <c r="D97">
         <v>0.0829524</v>
       </c>
-      <c r="E97" t="n">
+      <c r="E97">
         <v>0.9170476</v>
       </c>
-      <c r="F97" t="n">
+      <c r="F97">
         <v>7.244096665095901</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" t="n">
+    <row r="98" spans="1:6">
+      <c r="A98">
         <v>96</v>
       </c>
-      <c r="B98" t="n">
+      <c r="B98">
         <v>36155.82505103006</v>
       </c>
-      <c r="C98" t="n">
+      <c r="C98">
         <v>3243.022037029677</v>
       </c>
-      <c r="D98" t="n">
+      <c r="D98">
         <v>0.0896957</v>
       </c>
-      <c r="E98" t="n">
+      <c r="E98">
         <v>0.9103043</v>
       </c>
-      <c r="F98" t="n">
+      <c r="F98">
         <v>6.854140248658737</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="n">
+    <row r="99" spans="1:6">
+      <c r="A99">
         <v>97</v>
       </c>
-      <c r="B99" t="n">
+      <c r="B99">
         <v>32912.80301400038</v>
       </c>
-      <c r="C99" t="n">
+      <c r="C99">
         <v>3193.37458627429</v>
       </c>
-      <c r="D99" t="n">
+      <c r="D99">
         <v>0.09702529999999999</v>
       </c>
-      <c r="E99" t="n">
+      <c r="E99">
         <v>0.9029747</v>
       </c>
-      <c r="F99" t="n">
+      <c r="F99">
         <v>6.480237541071419</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" t="n">
+    <row r="100" spans="1:6">
+      <c r="A100">
         <v>98</v>
       </c>
-      <c r="B100" t="n">
+      <c r="B100">
         <v>29719.42842772608</v>
       </c>
-      <c r="C100" t="n">
+      <c r="C100">
         <v>3118.792482519689</v>
       </c>
-      <c r="D100" t="n">
+      <c r="D100">
         <v>0.1049412</v>
       </c>
-      <c r="E100" t="n">
+      <c r="E100">
         <v>0.8950588</v>
       </c>
-      <c r="F100" t="n">
+      <c r="F100">
         <v>6.122818492114362</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" t="n">
+    <row r="101" spans="1:6">
+      <c r="A101">
         <v>99</v>
       </c>
-      <c r="B101" t="n">
+      <c r="B101">
         <v>26600.6359452064</v>
       </c>
-      <c r="C101" t="n">
+      <c r="C101">
         <v>3017.669243850022</v>
       </c>
-      <c r="D101" t="n">
+      <c r="D101">
         <v>0.1134435</v>
       </c>
-      <c r="E101" t="n">
+      <c r="E101">
         <v>0.8865565</v>
       </c>
-      <c r="F101" t="n">
+      <c r="F101">
         <v>5.782066040928665</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" t="n">
+    <row r="102" spans="1:6">
+      <c r="A102">
         <v>100</v>
       </c>
-      <c r="B102" t="n">
+      <c r="B102">
         <v>23582.96670135638</v>
       </c>
-      <c r="C102" t="n">
+      <c r="C102">
         <v>2889.67279244394</v>
       </c>
-      <c r="D102" t="n">
+      <c r="D102">
         <v>0.1225322</v>
       </c>
-      <c r="E102" t="n">
+      <c r="E102">
         <v>0.8774678</v>
       </c>
-      <c r="F102" t="n">
+      <c r="F102">
         <v>5.457957604426414</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" t="n">
+    <row r="103" spans="1:6">
+      <c r="A103">
         <v>101</v>
       </c>
-      <c r="B103" t="n">
+      <c r="B103">
         <v>20693.29390891244</v>
       </c>
-      <c r="C103" t="n">
+      <c r="C103">
         <v>2735.800377144978</v>
       </c>
-      <c r="D103" t="n">
+      <c r="D103">
         <v>0.1322071</v>
       </c>
-      <c r="E103" t="n">
+      <c r="E103">
         <v>0.8677929</v>
       </c>
-      <c r="F103" t="n">
+      <c r="F103">
         <v>5.15030147479647</v>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" t="n">
+    <row r="104" spans="1:6">
+      <c r="A104">
         <v>102</v>
       </c>
-      <c r="B104" t="n">
+      <c r="B104">
         <v>17957.49353176746</v>
       </c>
-      <c r="C104" t="n">
+      <c r="C104">
         <v>2558.375371481259</v>
       </c>
-      <c r="D104" t="n">
+      <c r="D104">
         <v>0.1424684</v>
       </c>
-      <c r="E104" t="n">
+      <c r="E104">
         <v>0.8575315999999999</v>
       </c>
-      <c r="F104" t="n">
+      <c r="F104">
         <v>4.858768750927174</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" t="n">
+    <row r="105" spans="1:6">
+      <c r="A105">
         <v>103</v>
       </c>
-      <c r="B105" t="n">
+      <c r="B105">
         <v>15399.1181602862</v>
       </c>
-      <c r="C105" t="n">
+      <c r="C105">
         <v>2360.931199862439</v>
       </c>
-      <c r="D105" t="n">
+      <c r="D105">
         <v>0.153316</v>
       </c>
-      <c r="E105" t="n">
+      <c r="E105">
         <v>0.846684</v>
       </c>
-      <c r="F105" t="n">
+      <c r="F105">
         <v>4.58292493352685</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" t="n">
+    <row r="106" spans="1:6">
+      <c r="A106">
         <v>104</v>
       </c>
-      <c r="B106" t="n">
+      <c r="B106">
         <v>13038.18696042376</v>
       </c>
-      <c r="C106" t="n">
+      <c r="C106">
         <v>2148.041301729815</v>
       </c>
-      <c r="D106" t="n">
+      <c r="D106">
         <v>0.16475</v>
       </c>
-      <c r="E106" t="n">
+      <c r="E106">
         <v>0.83525</v>
       </c>
-      <c r="F106" t="n">
+      <c r="F106">
         <v>4.322253560391894</v>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" t="n">
+    <row r="107" spans="1:6">
+      <c r="A107">
         <v>105</v>
       </c>
-      <c r="B107" t="n">
+      <c r="B107">
         <v>10890.14565869395</v>
       </c>
-      <c r="C107" t="n">
+      <c r="C107">
         <v>1925.054315131026</v>
       </c>
-      <c r="D107" t="n">
+      <c r="D107">
         <v>0.1767703</v>
       </c>
-      <c r="E107" t="n">
+      <c r="E107">
         <v>0.8232297</v>
       </c>
-      <c r="F107" t="n">
+      <c r="F107">
         <v>4.076179060630822</v>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" t="n">
+    <row r="108" spans="1:6">
+      <c r="A108">
         <v>106</v>
       </c>
-      <c r="B108" t="n">
+      <c r="B108">
         <v>8965.091343562919</v>
       </c>
-      <c r="C108" t="n">
+      <c r="C108">
         <v>1697.78120686078</v>
       </c>
-      <c r="D108" t="n">
+      <c r="D108">
         <v>0.1893769</v>
       </c>
-      <c r="E108" t="n">
+      <c r="E108">
         <v>0.8106231</v>
       </c>
-      <c r="F108" t="n">
+      <c r="F108">
         <v>3.844084112406079</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" t="n">
+    <row r="109" spans="1:6">
+      <c r="A109">
         <v>107</v>
       </c>
-      <c r="B109" t="n">
+      <c r="B109">
         <v>7267.310136702139</v>
       </c>
-      <c r="C109" t="n">
+      <c r="C109">
         <v>1472.138287660739</v>
       </c>
-      <c r="D109" t="n">
+      <c r="D109">
         <v>0.2025699</v>
       </c>
-      <c r="E109" t="n">
+      <c r="E109">
         <v>0.7974301</v>
       </c>
-      <c r="F109" t="n">
+      <c r="F109">
         <v>3.625325459397935</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" t="n">
+    <row r="110" spans="1:6">
+      <c r="A110">
         <v>108</v>
       </c>
-      <c r="B110" t="n">
+      <c r="B110">
         <v>5795.1718490414</v>
       </c>
-      <c r="C110" t="n">
+      <c r="C110">
         <v>1253.780793402628</v>
       </c>
-      <c r="D110" t="n">
+      <c r="D110">
         <v>0.2163492</v>
       </c>
-      <c r="E110" t="n">
+      <c r="E110">
         <v>0.7836508</v>
       </c>
-      <c r="F110" t="n">
+      <c r="F110">
         <v>3.419246915056172</v>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" t="n">
+    <row r="111" spans="1:6">
+      <c r="A111">
         <v>109</v>
       </c>
-      <c r="B111" t="n">
+      <c r="B111">
         <v>4541.391055638773</v>
       </c>
-      <c r="C111" t="n">
+      <c r="C111">
         <v>1047.766129123488</v>
       </c>
-      <c r="D111" t="n">
+      <c r="D111">
         <v>0.2307148</v>
       </c>
-      <c r="E111" t="n">
+      <c r="E111">
         <v>0.7692852</v>
       </c>
-      <c r="F111" t="n">
+      <c r="F111">
         <v>3.225188457736753</v>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" t="n">
+    <row r="112" spans="1:6">
+      <c r="A112">
         <v>110</v>
       </c>
-      <c r="B112" t="n">
+      <c r="B112">
         <v>3493.624926515285</v>
       </c>
-      <c r="C112" t="n">
+      <c r="C112">
         <v>858.2676560972451</v>
       </c>
-      <c r="D112" t="n">
+      <c r="D112">
         <v>0.2456668</v>
       </c>
-      <c r="E112" t="n">
+      <c r="E112">
         <v>0.7543332</v>
       </c>
-      <c r="F112" t="n">
+      <c r="F112">
         <v>3.042494328159117</v>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" t="n">
+    <row r="113" spans="1:6">
+      <c r="A113">
         <v>111</v>
       </c>
-      <c r="B113" t="n">
+      <c r="B113">
         <v>2635.35727041804</v>
       </c>
-      <c r="C113" t="n">
+      <c r="C113">
         <v>688.3687593552712</v>
       </c>
-      <c r="D113" t="n">
+      <c r="D113">
         <v>0.2612051</v>
       </c>
-      <c r="E113" t="n">
+      <c r="E113">
         <v>0.7387949</v>
       </c>
-      <c r="F113" t="n">
+      <c r="F113">
         <v>2.870518927390598</v>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" t="n">
+    <row r="114" spans="1:6">
+      <c r="A114">
         <v>112</v>
       </c>
-      <c r="B114" t="n">
+      <c r="B114">
         <v>1946.988511062769</v>
       </c>
-      <c r="C114" t="n">
+      <c r="C114">
         <v>539.9577396764843</v>
       </c>
-      <c r="D114" t="n">
+      <c r="D114">
         <v>0.2773297</v>
       </c>
-      <c r="E114" t="n">
+      <c r="E114">
         <v>0.7226703</v>
       </c>
-      <c r="F114" t="n">
+      <c r="F114">
         <v>2.708629252030026</v>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" t="n">
+    <row r="115" spans="1:6">
+      <c r="A115">
         <v>113</v>
       </c>
-      <c r="B115" t="n">
+      <c r="B115">
         <v>1407.030771386284</v>
       </c>
-      <c r="C115" t="n">
+      <c r="C115">
         <v>413.7243129399629</v>
       </c>
-      <c r="D115" t="n">
+      <c r="D115">
         <v>0.2940407</v>
       </c>
-      <c r="E115" t="n">
+      <c r="E115">
         <v>0.7059593</v>
       </c>
-      <c r="F115" t="n">
+      <c r="F115">
         <v>2.556205924098481</v>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" t="n">
+    <row r="116" spans="1:6">
+      <c r="A116">
         <v>114</v>
       </c>
-      <c r="B116" t="n">
+      <c r="B116">
         <v>993.3064584463211</v>
       </c>
-      <c r="C116" t="n">
+      <c r="C116">
         <v>309.2540461597607</v>
       </c>
-      <c r="D116" t="n">
+      <c r="D116">
         <v>0.311338</v>
       </c>
-      <c r="E116" t="n">
+      <c r="E116">
         <v>0.688662</v>
       </c>
-      <c r="F116" t="n">
+      <c r="F116">
         <v>2.412640890343794</v>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" t="n">
+    <row r="117" spans="1:6">
+      <c r="A117">
         <v>115</v>
       </c>
-      <c r="B117" t="n">
+      <c r="B117">
         <v>684.0524122865604</v>
       </c>
-      <c r="C117" t="n">
+      <c r="C117">
         <v>225.2048980620823</v>
       </c>
-      <c r="D117" t="n">
+      <c r="D117">
         <v>0.3292217</v>
       </c>
-      <c r="E117" t="n">
+      <c r="E117">
         <v>0.6707783</v>
       </c>
-      <c r="F117" t="n">
+      <c r="F117">
         <v>2.27732892237962</v>
       </c>
     </row>
-    <row r="118">
-      <c r="A118" t="n">
+    <row r="118" spans="1:6">
+      <c r="A118">
         <v>116</v>
       </c>
-      <c r="B118" t="n">
+      <c r="B118">
         <v>458.8475142244781</v>
       </c>
-      <c r="C118" t="n">
+      <c r="C118">
         <v>159.5374263767316</v>
       </c>
-      <c r="D118" t="n">
+      <c r="D118">
         <v>0.3476916</v>
       </c>
-      <c r="E118" t="n">
+      <c r="E118">
         <v>0.6523084</v>
       </c>
-      <c r="F118" t="n">
+      <c r="F118">
         <v>2.149651788645548</v>
       </c>
     </row>
-    <row r="119">
-      <c r="A119" t="n">
+    <row r="119" spans="1:6">
+      <c r="A119">
         <v>117</v>
       </c>
-      <c r="B119" t="n">
+      <c r="B119">
         <v>299.3100878477466</v>
       </c>
-      <c r="C119" t="n">
+      <c r="C119">
         <v>109.7713760979854</v>
       </c>
-      <c r="D119" t="n">
+      <c r="D119">
         <v>0.366748</v>
       </c>
-      <c r="E119" t="n">
+      <c r="E119">
         <v>0.6332519999999999</v>
       </c>
-      <c r="F119" t="n">
+      <c r="F119">
         <v>2.028944573832788</v>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" t="n">
+    <row r="120" spans="1:6">
+      <c r="A120">
         <v>118</v>
       </c>
-      <c r="B120" t="n">
+      <c r="B120">
         <v>189.5387117497612</v>
       </c>
-      <c r="C120" t="n">
+      <c r="C120">
         <v>73.23597655621727</v>
       </c>
-      <c r="D120" t="n">
+      <c r="D120">
         <v>0.3863906</v>
       </c>
-      <c r="E120" t="n">
+      <c r="E120">
         <v>0.6136094000000001</v>
       </c>
-      <c r="F120" t="n">
+      <c r="F120">
         <v>1.914433075351973</v>
       </c>
     </row>
-    <row r="121">
-      <c r="A121" t="n">
+    <row r="121" spans="1:6">
+      <c r="A121">
         <v>119</v>
       </c>
-      <c r="B121" t="n">
+      <c r="B121">
         <v>116.3027351935439</v>
       </c>
-      <c r="C121" t="n">
+      <c r="C121">
         <v>47.29097166330476</v>
       </c>
-      <c r="D121" t="n">
+      <c r="D121">
         <v>0.4066196</v>
       </c>
-      <c r="E121" t="n">
+      <c r="E121">
         <v>0.5933804</v>
       </c>
-      <c r="F121" t="n">
+      <c r="F121">
         <v>1.80510333666983</v>
       </c>
     </row>
-    <row r="122">
-      <c r="A122" t="n">
+    <row r="122" spans="1:6">
+      <c r="A122">
         <v>120</v>
       </c>
-      <c r="B122" t="n">
+      <c r="B122">
         <v>69.01176353023918</v>
       </c>
-      <c r="C122" t="n">
+      <c r="C122">
         <v>29.49803624337143</v>
       </c>
-      <c r="D122" t="n">
+      <c r="D122">
         <v>0.4274349</v>
       </c>
-      <c r="E122" t="n">
+      <c r="E122">
         <v>0.5725651</v>
       </c>
-      <c r="F122" t="n">
+      <c r="F122">
         <v>1.699437892909557</v>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" t="n">
+    <row r="123" spans="1:6">
+      <c r="A123">
         <v>121</v>
       </c>
-      <c r="B123" t="n">
+      <c r="B123">
         <v>39.51372728686775</v>
       </c>
-      <c r="C123" t="n">
+      <c r="C123">
         <v>17.73520700876495</v>
       </c>
-      <c r="D123" t="n">
+      <c r="D123">
         <v>0.4488366</v>
       </c>
-      <c r="E123" t="n">
+      <c r="E123">
         <v>0.5511634000000001</v>
       </c>
-      <c r="F123" t="n">
+      <c r="F123">
         <v>1.594849813426555</v>
       </c>
     </row>
-    <row r="124">
-      <c r="A124" t="n">
+    <row r="124" spans="1:6">
+      <c r="A124">
         <v>122</v>
       </c>
-      <c r="B124" t="n">
+      <c r="B124">
         <v>21.77852027810281</v>
       </c>
-      <c r="C124" t="n">
+      <c r="C124">
         <v>10.25386309852964</v>
       </c>
-      <c r="D124" t="n">
+      <c r="D124">
         <v>0.4708246</v>
       </c>
-      <c r="E124" t="n">
+      <c r="E124">
         <v>0.5291754</v>
       </c>
-      <c r="F124" t="n">
+      <c r="F124">
         <v>1.486434174378333</v>
       </c>
     </row>
-    <row r="125">
-      <c r="A125" t="n">
+    <row r="125" spans="1:6">
+      <c r="A125">
         <v>123</v>
       </c>
-      <c r="B125" t="n">
+      <c r="B125">
         <v>11.52465717957316</v>
       </c>
-      <c r="C125" t="n">
+      <c r="C125">
         <v>5.686253175278501</v>
       </c>
-      <c r="D125" t="n">
+      <c r="D125">
         <v>0.4933989</v>
       </c>
-      <c r="E125" t="n">
+      <c r="E125">
         <v>0.5066011</v>
       </c>
-      <c r="F125" t="n">
+      <c r="F125">
         <v>1.364096808692039</v>
       </c>
     </row>
-    <row r="126">
-      <c r="A126" t="n">
+    <row r="126" spans="1:6">
+      <c r="A126">
         <v>124</v>
       </c>
-      <c r="B126" t="n">
+      <c r="B126">
         <v>5.838404004294662</v>
       </c>
-      <c r="C126" t="n">
+      <c r="C126">
         <v>3.015883053256448</v>
       </c>
-      <c r="D126" t="n">
+      <c r="D126">
         <v>0.5165594999999999</v>
       </c>
-      <c r="E126" t="n">
+      <c r="E126">
         <v>0.4834405000000001</v>
       </c>
-      <c r="F126" t="n">
+      <c r="F126">
         <v>1.20567495548675</v>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" t="n">
+    <row r="127" spans="1:6">
+      <c r="A127">
         <v>125</v>
       </c>
-      <c r="B127" t="n">
+      <c r="B127">
         <v>2.822520951038214</v>
       </c>
-      <c r="C127" t="n">
+      <c r="C127">
         <v>1.525026416232129</v>
       </c>
-      <c r="D127" t="n">
+      <c r="D127">
         <v>0.5403065</v>
       </c>
-      <c r="E127" t="n">
+      <c r="E127">
         <v>0.4596935</v>
       </c>
-      <c r="F127" t="n">
+      <c r="F127">
         <v>0.9596935</v>
       </c>
     </row>
-    <row r="128">
-      <c r="A128" t="n">
+    <row r="128" spans="1:6">
+      <c r="A128">
         <v>126</v>
       </c>
-      <c r="B128" t="n">
+      <c r="B128">
         <v>1.297494534806085</v>
       </c>
-      <c r="C128" t="n">
+      <c r="C128">
         <v>1.297494534806085</v>
       </c>
-      <c r="D128" t="n">
+      <c r="D128">
         <v>1</v>
       </c>
-      <c r="E128" t="n">
-        <v>0</v>
-      </c>
-      <c r="F128" t="n">
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
         <v>0.5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>